<commit_message>
Edit Sprint III Backlog and BurndownChart
</commit_message>
<xml_diff>
--- a/Sprint3/Sprint_III_BurndownChart.xlsx
+++ b/Sprint3/Sprint_III_BurndownChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\SprintIII\Sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Sprint_III\Team_Software_Engineer\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4835301F-BCAF-43E2-B0C2-A5FFBEBB5A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92EFF79-D1AB-4A90-9086-5E26F2BA31DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>SprintBurndown Chart</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>นาย ธนพงษ์ เจริญพันธ์</t>
+  </si>
+  <si>
+    <t>User Manual For Customer</t>
+  </si>
+  <si>
+    <t>User Manual For Admin</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Slide Present</t>
+  </si>
+  <si>
+    <t>3 &amp; 6</t>
   </si>
 </sst>
 </file>
@@ -400,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -949,11 +964,294 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1148,17 +1446,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,6 +1466,11 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1188,21 +1490,118 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -2111,22 +2510,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2209,22 +2608,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.166666666666664</c:v>
+                  <c:v>44.166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.333333333333332</c:v>
+                  <c:v>35.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.5</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.666666666666666</c:v>
+                  <c:v>17.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.833333333333333</c:v>
+                  <c:v>8.8333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3293,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24:Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
@@ -3312,32 +3711,32 @@
   <sheetData>
     <row r="1" spans="2:34" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:34" ht="25.5" customHeight="1">
-      <c r="B2" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="95"/>
+      <c r="B2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B3" s="96"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="98"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="102"/>
       <c r="W3" s="74"/>
       <c r="X3" s="74"/>
       <c r="Y3" s="74"/>
@@ -3378,13 +3777,13 @@
       <c r="AH4" s="15"/>
     </row>
     <row r="5" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="105" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -3427,9 +3826,9 @@
       <c r="AH5" s="15"/>
     </row>
     <row r="6" spans="2:34" ht="15" customHeight="1">
-      <c r="B6" s="100"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
       <c r="E6" s="16" t="s">
         <v>5</v>
       </c>
@@ -3472,10 +3871,10 @@
       <c r="AH6" s="15"/>
     </row>
     <row r="7" spans="2:34" ht="15" customHeight="1">
-      <c r="B7" s="103">
+      <c r="B7" s="107">
         <v>1</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="108" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -3507,7 +3906,7 @@
       </c>
       <c r="M7" s="15"/>
       <c r="V7" s="15"/>
-      <c r="W7" s="82">
+      <c r="W7" s="111">
         <v>1</v>
       </c>
       <c r="X7" s="52" t="s">
@@ -3543,8 +3942,8 @@
       <c r="AH7" s="15"/>
     </row>
     <row r="8" spans="2:34" ht="15" customHeight="1">
-      <c r="B8" s="104"/>
-      <c r="C8" s="107"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="109"/>
       <c r="D8" s="18" t="s">
         <v>18</v>
       </c>
@@ -3574,7 +3973,7 @@
       </c>
       <c r="M8" s="15"/>
       <c r="V8" s="15"/>
-      <c r="W8" s="83"/>
+      <c r="W8" s="96"/>
       <c r="X8" s="52"/>
       <c r="Y8" s="75">
         <v>4</v>
@@ -3607,8 +4006,8 @@
       <c r="AH8" s="15"/>
     </row>
     <row r="9" spans="2:34" ht="15" customHeight="1">
-      <c r="B9" s="104"/>
-      <c r="C9" s="107"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="109"/>
       <c r="D9" s="18" t="s">
         <v>19</v>
       </c>
@@ -3638,7 +4037,7 @@
       </c>
       <c r="M9" s="15"/>
       <c r="V9" s="15"/>
-      <c r="W9" s="84">
+      <c r="W9" s="112">
         <v>5</v>
       </c>
       <c r="X9" s="52" t="s">
@@ -3658,8 +4057,8 @@
       <c r="AH9" s="15"/>
     </row>
     <row r="10" spans="2:34" ht="15" customHeight="1">
-      <c r="B10" s="104"/>
-      <c r="C10" s="107"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="18" t="s">
         <v>21</v>
       </c>
@@ -3689,7 +4088,7 @@
       </c>
       <c r="M10" s="15"/>
       <c r="V10" s="15"/>
-      <c r="W10" s="83"/>
+      <c r="W10" s="96"/>
       <c r="X10" s="52"/>
       <c r="Y10" s="75">
         <v>4</v>
@@ -3705,8 +4104,8 @@
       <c r="AH10" s="15"/>
     </row>
     <row r="11" spans="2:34" ht="15" customHeight="1">
-      <c r="B11" s="104"/>
-      <c r="C11" s="107"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="109"/>
       <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
@@ -3756,8 +4155,8 @@
       <c r="AH11" s="15"/>
     </row>
     <row r="12" spans="2:34" ht="15" customHeight="1">
-      <c r="B12" s="104"/>
-      <c r="C12" s="107"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="109"/>
       <c r="D12" s="18" t="s">
         <v>24</v>
       </c>
@@ -3807,8 +4206,8 @@
       <c r="AH12" s="15"/>
     </row>
     <row r="13" spans="2:34" ht="15" customHeight="1">
-      <c r="B13" s="104"/>
-      <c r="C13" s="107"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="109"/>
       <c r="D13" s="18" t="s">
         <v>26</v>
       </c>
@@ -3858,8 +4257,8 @@
       <c r="AH13" s="15"/>
     </row>
     <row r="14" spans="2:34" ht="15" customHeight="1">
-      <c r="B14" s="104"/>
-      <c r="C14" s="107"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="109"/>
       <c r="D14" s="18" t="s">
         <v>27</v>
       </c>
@@ -3909,8 +4308,8 @@
       <c r="AH14" s="15"/>
     </row>
     <row r="15" spans="2:34" ht="15" customHeight="1">
-      <c r="B15" s="104"/>
-      <c r="C15" s="107"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="109"/>
       <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
@@ -3960,8 +4359,8 @@
       <c r="AH15" s="15"/>
     </row>
     <row r="16" spans="2:34" ht="15" customHeight="1">
-      <c r="B16" s="104"/>
-      <c r="C16" s="107"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="18" t="s">
         <v>29</v>
       </c>
@@ -4011,8 +4410,8 @@
       <c r="AH16" s="15"/>
     </row>
     <row r="17" spans="2:34" ht="15" customHeight="1">
-      <c r="B17" s="104"/>
-      <c r="C17" s="107"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="18" t="s">
         <v>30</v>
       </c>
@@ -4062,8 +4461,8 @@
       <c r="AH17" s="15"/>
     </row>
     <row r="18" spans="2:34" ht="15" customHeight="1">
-      <c r="B18" s="104"/>
-      <c r="C18" s="107"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="22" t="s">
         <v>32</v>
       </c>
@@ -4113,8 +4512,8 @@
       <c r="AH18" s="15"/>
     </row>
     <row r="19" spans="2:34" ht="15" customHeight="1">
-      <c r="B19" s="104"/>
-      <c r="C19" s="107"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="22" t="s">
         <v>34</v>
       </c>
@@ -4164,8 +4563,8 @@
       <c r="AH19" s="15"/>
     </row>
     <row r="20" spans="2:34" ht="15" customHeight="1">
-      <c r="B20" s="104"/>
-      <c r="C20" s="107"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="109"/>
       <c r="D20" s="22" t="s">
         <v>35</v>
       </c>
@@ -4215,8 +4614,8 @@
       <c r="AH20" s="15"/>
     </row>
     <row r="21" spans="2:34" ht="15" customHeight="1">
-      <c r="B21" s="105"/>
-      <c r="C21" s="108"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="110"/>
       <c r="D21" s="23" t="s">
         <v>37</v>
       </c>
@@ -4266,11 +4665,11 @@
       <c r="AH21" s="15"/>
     </row>
     <row r="22" spans="2:34" ht="15" customHeight="1">
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="90"/>
       <c r="E22" s="26">
         <f t="shared" ref="E22:L22" si="0">SUM(E7:E21)</f>
         <v>86</v>
@@ -4329,11 +4728,11 @@
       <c r="AH22" s="15"/>
     </row>
     <row r="23" spans="2:34" ht="15" customHeight="1">
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="91"/>
-      <c r="D23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="28">
         <f>SUM(E7:E21)</f>
         <v>86</v>
@@ -4383,10 +4782,10 @@
       <c r="AH23" s="15"/>
     </row>
     <row r="24" spans="2:34" ht="15" customHeight="1">
-      <c r="B24" s="109">
+      <c r="B24" s="82">
         <v>2</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="C24" s="85" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="31" t="s">
@@ -4418,7 +4817,7 @@
       </c>
       <c r="M24" s="15"/>
       <c r="V24" s="15"/>
-      <c r="W24" s="85">
+      <c r="W24" s="94">
         <v>4</v>
       </c>
       <c r="X24" s="40" t="s">
@@ -4454,8 +4853,8 @@
       <c r="AH24" s="15"/>
     </row>
     <row r="25" spans="2:34" ht="15" customHeight="1">
-      <c r="B25" s="104"/>
-      <c r="C25" s="111"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="35" t="s">
         <v>45</v>
       </c>
@@ -4485,7 +4884,7 @@
       </c>
       <c r="M25" s="15"/>
       <c r="V25" s="15"/>
-      <c r="W25" s="86"/>
+      <c r="W25" s="95"/>
       <c r="X25" s="40" t="s">
         <v>44</v>
       </c>
@@ -4527,8 +4926,8 @@
       <c r="AH25" s="15"/>
     </row>
     <row r="26" spans="2:34" ht="15" customHeight="1">
-      <c r="B26" s="104"/>
-      <c r="C26" s="111"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="35" t="s">
         <v>46</v>
       </c>
@@ -4558,7 +4957,7 @@
       </c>
       <c r="M26" s="15"/>
       <c r="V26" s="15"/>
-      <c r="W26" s="83"/>
+      <c r="W26" s="96"/>
       <c r="X26" s="40" t="s">
         <v>44</v>
       </c>
@@ -4576,8 +4975,8 @@
       <c r="AH26" s="15"/>
     </row>
     <row r="27" spans="2:34" ht="15" customHeight="1">
-      <c r="B27" s="104"/>
-      <c r="C27" s="111"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="35" t="s">
         <v>47</v>
       </c>
@@ -4627,8 +5026,8 @@
       <c r="AH27" s="15"/>
     </row>
     <row r="28" spans="2:34" ht="15" customHeight="1">
-      <c r="B28" s="104"/>
-      <c r="C28" s="111"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="35" t="s">
         <v>49</v>
       </c>
@@ -4678,8 +5077,8 @@
       <c r="AH28" s="15"/>
     </row>
     <row r="29" spans="2:34" ht="15" customHeight="1">
-      <c r="B29" s="104"/>
-      <c r="C29" s="111"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="35" t="s">
         <v>50</v>
       </c>
@@ -4729,8 +5128,8 @@
       <c r="AH29" s="15"/>
     </row>
     <row r="30" spans="2:34" ht="15" customHeight="1">
-      <c r="B30" s="104"/>
-      <c r="C30" s="111"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="35" t="s">
         <v>52</v>
       </c>
@@ -4782,8 +5181,8 @@
       <c r="AH30" s="15"/>
     </row>
     <row r="31" spans="2:34" ht="15" customHeight="1">
-      <c r="B31" s="104"/>
-      <c r="C31" s="111"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="35" t="s">
         <v>55</v>
       </c>
@@ -4833,8 +5232,8 @@
       <c r="AH31" s="15"/>
     </row>
     <row r="32" spans="2:34" ht="15" customHeight="1">
-      <c r="B32" s="104"/>
-      <c r="C32" s="111"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="35" t="s">
         <v>56</v>
       </c>
@@ -4884,8 +5283,8 @@
       <c r="AH32" s="15"/>
     </row>
     <row r="33" spans="2:34" ht="15" customHeight="1">
-      <c r="B33" s="104"/>
-      <c r="C33" s="111"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="41"/>
       <c r="E33" s="42"/>
       <c r="F33" s="43"/>
@@ -4911,8 +5310,8 @@
       <c r="AH33" s="15"/>
     </row>
     <row r="34" spans="2:34" ht="15" customHeight="1">
-      <c r="B34" s="104"/>
-      <c r="C34" s="111"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="86"/>
       <c r="D34" s="45"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
@@ -4938,8 +5337,8 @@
       <c r="AH34" s="15"/>
     </row>
     <row r="35" spans="2:34" ht="15" customHeight="1">
-      <c r="B35" s="104"/>
-      <c r="C35" s="111"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="86"/>
       <c r="D35" s="22"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -4965,8 +5364,8 @@
       <c r="AH35" s="15"/>
     </row>
     <row r="36" spans="2:34" ht="15" customHeight="1">
-      <c r="B36" s="104"/>
-      <c r="C36" s="111"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="86"/>
       <c r="D36" s="22"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
@@ -4992,8 +5391,8 @@
       <c r="AH36" s="15"/>
     </row>
     <row r="37" spans="2:34" ht="15" customHeight="1">
-      <c r="B37" s="104"/>
-      <c r="C37" s="111"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="86"/>
       <c r="D37" s="22"/>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
@@ -5019,8 +5418,8 @@
       <c r="AH37" s="15"/>
     </row>
     <row r="38" spans="2:34" ht="15" customHeight="1">
-      <c r="B38" s="105"/>
-      <c r="C38" s="112"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="87"/>
       <c r="D38" s="23"/>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -5046,11 +5445,11 @@
       <c r="AH38" s="15"/>
     </row>
     <row r="39" spans="2:34" ht="15" customHeight="1" thickBot="1">
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="88"/>
-      <c r="D39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="90"/>
       <c r="E39" s="48">
         <f t="shared" ref="E39:L39" si="2">SUM(E24:E38)</f>
         <v>35</v>
@@ -5109,43 +5508,43 @@
       <c r="AH39" s="15"/>
     </row>
     <row r="40" spans="2:34" ht="15" customHeight="1" thickBot="1">
-      <c r="B40" s="90" t="s">
+      <c r="B40" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="91"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="29">
+      <c r="C40" s="117"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="119">
         <f>E39</f>
         <v>35</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="119">
         <f>(E40/6)*5</f>
         <v>29.166666666666664</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="119">
         <f>(E40/6)*4</f>
         <v>23.333333333333332</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="119">
         <f>(E40/6)*3</f>
         <v>17.5</v>
       </c>
-      <c r="I40" s="29">
+      <c r="I40" s="119">
         <f>(E40/6)*2</f>
         <v>11.666666666666666</v>
       </c>
-      <c r="J40" s="29">
+      <c r="J40" s="119">
         <f>(E40/6)*1</f>
         <v>5.833333333333333</v>
       </c>
-      <c r="K40" s="29">
+      <c r="K40" s="119">
         <f>(E40/6)*0</f>
         <v>0</v>
       </c>
-      <c r="L40" s="30">
-        <v>0</v>
-      </c>
-      <c r="M40" s="15"/>
+      <c r="L40" s="120">
+        <v>0</v>
+      </c>
+      <c r="M40" s="121"/>
       <c r="W40" s="15"/>
       <c r="X40" s="15"/>
       <c r="Y40" s="62" t="s">
@@ -5162,47 +5561,48 @@
       <c r="AH40" s="74"/>
     </row>
     <row r="41" spans="2:34" ht="15" customHeight="1">
-      <c r="B41" s="109">
+      <c r="B41" s="127">
         <v>3</v>
       </c>
-      <c r="C41" s="110" t="s">
+      <c r="C41" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="32">
-        <v>1</v>
-      </c>
-      <c r="F41" s="37">
-        <v>0</v>
-      </c>
-      <c r="G41" s="37">
-        <v>0</v>
-      </c>
-      <c r="H41" s="37">
-        <v>0</v>
-      </c>
-      <c r="I41" s="37">
-        <v>0</v>
-      </c>
-      <c r="J41" s="37">
-        <v>0</v>
-      </c>
-      <c r="K41" s="37">
-        <v>0</v>
-      </c>
-      <c r="L41" s="34">
-        <v>0</v>
-      </c>
-      <c r="W41" s="85">
+      <c r="D41" s="137" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="138">
         <v>4</v>
       </c>
+      <c r="F41" s="139">
+        <v>4</v>
+      </c>
+      <c r="G41" s="139">
+        <v>4</v>
+      </c>
+      <c r="H41" s="139">
+        <v>4</v>
+      </c>
+      <c r="I41" s="139">
+        <v>4</v>
+      </c>
+      <c r="J41" s="139">
+        <v>4</v>
+      </c>
+      <c r="K41" s="139">
+        <v>0</v>
+      </c>
+      <c r="L41" s="140">
+        <v>0</v>
+      </c>
+      <c r="M41" s="129"/>
+      <c r="W41" s="57">
+        <v>5</v>
+      </c>
       <c r="X41" s="40" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="Y41" s="77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z41" s="63" t="s">
         <v>17</v>
@@ -5230,65 +5630,68 @@
       </c>
     </row>
     <row r="42" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B42" s="104"/>
-      <c r="C42" s="111"/>
-      <c r="D42" s="35" t="s">
-        <v>45</v>
+      <c r="B42" s="130"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="E42" s="36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F42" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G42" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H42" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I42" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J42" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K42" s="37">
         <v>0</v>
       </c>
-      <c r="L42" s="38">
-        <v>0</v>
-      </c>
-      <c r="W42" s="86"/>
+      <c r="L42" s="141">
+        <v>0</v>
+      </c>
+      <c r="M42" s="131"/>
+      <c r="W42" s="156">
+        <v>2</v>
+      </c>
       <c r="X42" s="40" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="Y42" s="77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z42" s="64">
         <f t="shared" ref="Z42" si="3">E56</f>
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="AA42" s="65">
         <f t="shared" ref="AA42" si="4">F56</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="AB42" s="65">
         <f t="shared" ref="AB42" si="5">G56</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="AC42" s="65">
         <f t="shared" ref="AC42" si="6">H56</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AD42" s="65">
         <f t="shared" ref="AD42" si="7">I56</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AE42" s="65">
         <f t="shared" ref="AE42" si="8">J56</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AF42" s="65">
         <f t="shared" ref="AF42" si="9">K56</f>
@@ -5300,19 +5703,19 @@
       </c>
     </row>
     <row r="43" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B43" s="104"/>
-      <c r="C43" s="111"/>
-      <c r="D43" s="35" t="s">
-        <v>46</v>
+      <c r="B43" s="130"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="E43" s="36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F43" s="37">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G43" s="37">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H43" s="37">
         <v>0</v>
@@ -5326,15 +5729,16 @@
       <c r="K43" s="37">
         <v>0</v>
       </c>
-      <c r="L43" s="38">
-        <v>0</v>
-      </c>
-      <c r="W43" s="83"/>
+      <c r="L43" s="142">
+        <v>0</v>
+      </c>
+      <c r="M43" s="131"/>
+      <c r="W43" s="156"/>
       <c r="X43" s="40" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="Y43" s="77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z43" s="67"/>
       <c r="AA43" s="22"/>
@@ -5346,43 +5750,44 @@
       <c r="AG43" s="54"/>
     </row>
     <row r="44" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B44" s="104"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="35" t="s">
-        <v>47</v>
+      <c r="B44" s="130"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="E44" s="36">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F44" s="37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G44" s="37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H44" s="37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I44" s="37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J44" s="37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K44" s="37">
         <v>0</v>
       </c>
-      <c r="L44" s="38">
-        <v>0</v>
-      </c>
-      <c r="W44" s="58">
-        <v>1</v>
-      </c>
-      <c r="X44" s="40" t="s">
-        <v>48</v>
+      <c r="L44" s="141">
+        <v>0</v>
+      </c>
+      <c r="M44" s="131"/>
+      <c r="W44" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="X44" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="Y44" s="77">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="Z44" s="67"/>
       <c r="AA44" s="22"/>
@@ -5394,19 +5799,19 @@
       <c r="AG44" s="54"/>
     </row>
     <row r="45" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B45" s="104"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="35" t="s">
-        <v>49</v>
+      <c r="B45" s="130"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="E45" s="36">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F45" s="37">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G45" s="37">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H45" s="37">
         <v>0</v>
@@ -5420,17 +5825,16 @@
       <c r="K45" s="37">
         <v>0</v>
       </c>
-      <c r="L45" s="39">
-        <v>0</v>
-      </c>
-      <c r="W45" s="60">
-        <v>2</v>
-      </c>
-      <c r="X45" s="40" t="s">
-        <v>33</v>
+      <c r="L45" s="142">
+        <v>0</v>
+      </c>
+      <c r="M45" s="131"/>
+      <c r="W45" s="157"/>
+      <c r="X45" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="Y45" s="77">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Z45" s="67"/>
       <c r="AA45" s="22"/>
@@ -5442,25 +5846,25 @@
       <c r="AG45" s="54"/>
     </row>
     <row r="46" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B46" s="104"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="35" t="s">
-        <v>50</v>
+      <c r="B46" s="130"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="E46" s="36">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F46" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G46" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H46" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I46" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J46" s="37">
         <v>0</v>
@@ -5468,20 +5872,21 @@
       <c r="K46" s="37">
         <v>0</v>
       </c>
-      <c r="L46" s="39">
-        <v>0</v>
-      </c>
+      <c r="L46" s="142">
+        <v>0</v>
+      </c>
+      <c r="M46" s="131"/>
       <c r="P46" s="7"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="8"/>
-      <c r="W46" s="68">
-        <v>6</v>
-      </c>
-      <c r="X46" s="15" t="s">
-        <v>51</v>
+      <c r="W46" s="56">
+        <v>4</v>
+      </c>
+      <c r="X46" s="155" t="s">
+        <v>44</v>
       </c>
       <c r="Y46" s="77">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Z46" s="67"/>
       <c r="AA46" s="22"/>
@@ -5493,22 +5898,22 @@
       <c r="AG46" s="54"/>
     </row>
     <row r="47" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B47" s="104"/>
-      <c r="C47" s="111"/>
-      <c r="D47" s="35" t="s">
-        <v>52</v>
+      <c r="B47" s="130"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="E47" s="36">
         <v>4</v>
       </c>
       <c r="F47" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G47" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H47" s="37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I47" s="37">
         <v>0</v>
@@ -5519,20 +5924,21 @@
       <c r="K47" s="37">
         <v>0</v>
       </c>
-      <c r="L47" s="39">
-        <v>0</v>
-      </c>
+      <c r="L47" s="142">
+        <v>0</v>
+      </c>
+      <c r="M47" s="131"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="8"/>
-      <c r="W47" s="69">
-        <v>3</v>
-      </c>
-      <c r="X47" s="15" t="s">
-        <v>54</v>
+      <c r="W47" s="57">
+        <v>5</v>
+      </c>
+      <c r="X47" s="52" t="s">
+        <v>20</v>
       </c>
       <c r="Y47" s="77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z47" s="67"/>
       <c r="AA47" s="22"/>
@@ -5544,46 +5950,47 @@
       <c r="AG47" s="54"/>
     </row>
     <row r="48" spans="2:34" ht="14.25" customHeight="1">
-      <c r="B48" s="104"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="36">
-        <v>6</v>
-      </c>
-      <c r="F48" s="37">
-        <v>0</v>
-      </c>
-      <c r="G48" s="37">
-        <v>0</v>
-      </c>
-      <c r="H48" s="37">
-        <v>0</v>
-      </c>
-      <c r="I48" s="37">
-        <v>0</v>
-      </c>
-      <c r="J48" s="37">
-        <v>0</v>
-      </c>
-      <c r="K48" s="37">
-        <v>0</v>
-      </c>
-      <c r="L48" s="38">
-        <v>0</v>
-      </c>
+      <c r="B48" s="130"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="143" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="144">
+        <v>4</v>
+      </c>
+      <c r="F48" s="145">
+        <v>4</v>
+      </c>
+      <c r="G48" s="145">
+        <v>4</v>
+      </c>
+      <c r="H48" s="145">
+        <v>4</v>
+      </c>
+      <c r="I48" s="145">
+        <v>0</v>
+      </c>
+      <c r="J48" s="145">
+        <v>0</v>
+      </c>
+      <c r="K48" s="145">
+        <v>0</v>
+      </c>
+      <c r="L48" s="146">
+        <v>0</v>
+      </c>
+      <c r="M48" s="131"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="8"/>
-      <c r="W48" s="70">
-        <v>5</v>
-      </c>
-      <c r="X48" s="15" t="s">
-        <v>20</v>
+      <c r="W48" s="58">
+        <v>1</v>
+      </c>
+      <c r="X48" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="Y48" s="77">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Z48" s="67"/>
       <c r="AA48" s="22"/>
@@ -5595,46 +6002,47 @@
       <c r="AG48" s="54"/>
     </row>
     <row r="49" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B49" s="104"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="36">
-        <v>4</v>
-      </c>
-      <c r="F49" s="37">
-        <v>0</v>
-      </c>
-      <c r="G49" s="37">
-        <v>0</v>
-      </c>
-      <c r="H49" s="37">
-        <v>0</v>
-      </c>
-      <c r="I49" s="37">
-        <v>0</v>
-      </c>
-      <c r="J49" s="37">
-        <v>0</v>
-      </c>
-      <c r="K49" s="37">
-        <v>0</v>
-      </c>
-      <c r="L49" s="39">
-        <v>0</v>
-      </c>
+      <c r="B49" s="130"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="151" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="152">
+        <v>3</v>
+      </c>
+      <c r="F49" s="153">
+        <v>3</v>
+      </c>
+      <c r="G49" s="153">
+        <v>3</v>
+      </c>
+      <c r="H49" s="153">
+        <v>3</v>
+      </c>
+      <c r="I49" s="153">
+        <v>3</v>
+      </c>
+      <c r="J49" s="153">
+        <v>3</v>
+      </c>
+      <c r="K49" s="153">
+        <v>0</v>
+      </c>
+      <c r="L49" s="154">
+        <v>0</v>
+      </c>
+      <c r="M49" s="131"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="8"/>
-      <c r="W49" s="68">
-        <v>6</v>
-      </c>
-      <c r="X49" s="15" t="s">
-        <v>31</v>
+      <c r="W49" s="56">
+        <v>4</v>
+      </c>
+      <c r="X49" s="155" t="s">
+        <v>44</v>
       </c>
       <c r="Y49" s="77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z49" s="67"/>
       <c r="AA49" s="22"/>
@@ -5646,17 +6054,18 @@
       <c r="AG49" s="54"/>
     </row>
     <row r="50" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B50" s="104"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="44"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="115"/>
+      <c r="K50" s="115"/>
+      <c r="L50" s="147"/>
+      <c r="M50" s="131"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="5"/>
       <c r="R50" s="8"/>
@@ -5673,8 +6082,8 @@
       <c r="AG50" s="54"/>
     </row>
     <row r="51" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B51" s="104"/>
-      <c r="C51" s="111"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="86"/>
       <c r="D51" s="45"/>
       <c r="E51" s="46"/>
       <c r="F51" s="46"/>
@@ -5683,7 +6092,8 @@
       <c r="I51" s="46"/>
       <c r="J51" s="46"/>
       <c r="K51" s="46"/>
-      <c r="L51" s="47"/>
+      <c r="L51" s="148"/>
+      <c r="M51" s="131"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="5"/>
       <c r="R51" s="8"/>
@@ -5700,8 +6110,8 @@
       <c r="AG51" s="54"/>
     </row>
     <row r="52" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B52" s="104"/>
-      <c r="C52" s="111"/>
+      <c r="B52" s="130"/>
+      <c r="C52" s="86"/>
       <c r="D52" s="22"/>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
@@ -5710,7 +6120,8 @@
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
-      <c r="L52" s="21"/>
+      <c r="L52" s="149"/>
+      <c r="M52" s="131"/>
       <c r="W52" s="15"/>
       <c r="X52" s="15"/>
       <c r="Y52" s="78"/>
@@ -5724,8 +6135,8 @@
       <c r="AG52" s="54"/>
     </row>
     <row r="53" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B53" s="104"/>
-      <c r="C53" s="111"/>
+      <c r="B53" s="130"/>
+      <c r="C53" s="86"/>
       <c r="D53" s="22"/>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
@@ -5734,7 +6145,8 @@
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
-      <c r="L53" s="21"/>
+      <c r="L53" s="149"/>
+      <c r="M53" s="131"/>
       <c r="W53" s="15"/>
       <c r="X53" s="15"/>
       <c r="Y53" s="78"/>
@@ -5748,8 +6160,8 @@
       <c r="AG53" s="54"/>
     </row>
     <row r="54" spans="2:33" ht="14.25" customHeight="1">
-      <c r="B54" s="104"/>
-      <c r="C54" s="111"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="86"/>
       <c r="D54" s="22"/>
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
@@ -5758,7 +6170,8 @@
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
       <c r="K54" s="20"/>
-      <c r="L54" s="21"/>
+      <c r="L54" s="149"/>
+      <c r="M54" s="131"/>
       <c r="W54" s="15"/>
       <c r="X54" s="15"/>
       <c r="Y54" s="78"/>
@@ -5772,17 +6185,18 @@
       <c r="AG54" s="54"/>
     </row>
     <row r="55" spans="2:33" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B55" s="105"/>
-      <c r="C55" s="112"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="25"/>
+      <c r="B55" s="132"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="134"/>
+      <c r="E55" s="135"/>
+      <c r="F55" s="135"/>
+      <c r="G55" s="135"/>
+      <c r="H55" s="135"/>
+      <c r="I55" s="135"/>
+      <c r="J55" s="135"/>
+      <c r="K55" s="135"/>
+      <c r="L55" s="150"/>
+      <c r="M55" s="136"/>
       <c r="W55" s="15"/>
       <c r="X55" s="15"/>
       <c r="Y55" s="78"/>
@@ -5796,57 +6210,58 @@
       <c r="AG55" s="71"/>
     </row>
     <row r="56" spans="2:33" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B56" s="87" t="s">
+      <c r="B56" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="88"/>
-      <c r="D56" s="89"/>
-      <c r="E56" s="48">
-        <f t="shared" ref="E56:L56" si="11">SUM(E41:E55)</f>
-        <v>35</v>
-      </c>
-      <c r="F56" s="48">
+      <c r="C56" s="123"/>
+      <c r="D56" s="124"/>
+      <c r="E56" s="125">
+        <f>SUM(E41:E55)</f>
+        <v>53</v>
+      </c>
+      <c r="F56" s="125">
+        <f>SUM(F41:F55)</f>
+        <v>53</v>
+      </c>
+      <c r="G56" s="125">
+        <f t="shared" ref="E56:L56" si="11">SUM(G41:G55)</f>
+        <v>53</v>
+      </c>
+      <c r="H56" s="125">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G56" s="48">
+        <v>39</v>
+      </c>
+      <c r="I56" s="125">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H56" s="48">
+        <v>31</v>
+      </c>
+      <c r="J56" s="125">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I56" s="48">
+        <v>27</v>
+      </c>
+      <c r="K56" s="125">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J56" s="48">
+      <c r="L56" s="125">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K56" s="48">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="L56" s="48">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+      <c r="M56" s="126"/>
       <c r="W56" s="15"/>
       <c r="X56" s="52" t="s">
         <v>39</v>
       </c>
       <c r="Y56" s="80">
         <f>SUM(Y41:Y55)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Z56" s="23" t="s">
         <v>40</v>
       </c>
       <c r="AA56" s="23">
-        <f>(Z25+Z42)/2</f>
-        <v>35</v>
+        <f>(Z25+Z42+Z8)/3</f>
+        <v>58</v>
       </c>
       <c r="AB56" s="23"/>
       <c r="AC56" s="23"/>
@@ -5856,34 +6271,34 @@
       <c r="AG56" s="73"/>
     </row>
     <row r="57" spans="2:33" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B57" s="90" t="s">
+      <c r="B57" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="C57" s="91"/>
-      <c r="D57" s="92"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="93"/>
       <c r="E57" s="29">
         <f>E56</f>
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="F57" s="29">
         <f>(E57/6)*5</f>
-        <v>29.166666666666664</v>
+        <v>44.166666666666671</v>
       </c>
       <c r="G57" s="29">
         <f>(E57/6)*4</f>
-        <v>23.333333333333332</v>
+        <v>35.333333333333336</v>
       </c>
       <c r="H57" s="29">
         <f>(E57/6)*3</f>
-        <v>17.5</v>
+        <v>26.5</v>
       </c>
       <c r="I57" s="29">
         <f>(E57/6)*2</f>
-        <v>11.666666666666666</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="J57" s="29">
         <f>(E57/6)*1</f>
-        <v>5.833333333333333</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="K57" s="29">
         <f>(E57/6)*0</f>
@@ -6950,18 +7365,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B41:B55"/>
-    <mergeCell ref="C41:C55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="W41:W43"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B7:B21"/>
-    <mergeCell ref="C7:C21"/>
+  <mergeCells count="21">
     <mergeCell ref="W7:W8"/>
     <mergeCell ref="W9:W10"/>
     <mergeCell ref="W24:W26"/>
@@ -6971,6 +7375,18 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:B38"/>
     <mergeCell ref="C24:C38"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B7:B21"/>
+    <mergeCell ref="C7:C21"/>
+    <mergeCell ref="B41:B55"/>
+    <mergeCell ref="C41:C55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="W42:W43"/>
+    <mergeCell ref="W44:W45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>